<commit_message>
feat(dictionaries): add Payments Report page
- New API endpoint /api/payments-report for aggregated payment data
- PaymentsReportTable component with filtering, sorting, and totals
- Shows Counteragent, Payment ID, Financial Code, Currency, Project, Job
- Displays aggregated Accrual, Order, Balance, Accrual/Floor metrics
- Added to dictionaries navigation menu
</commit_message>
<xml_diff>
--- a/templates/paymentledger_import_template.xlsx
+++ b/templates/paymentledger_import_template.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Paymentledger" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Paymentledger" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,10 +456,15 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>recordUuid</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>userEmail</t>
         </is>
@@ -473,7 +478,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-12-24 20:06:31</t>
+          <t>2026-01-05 00:22:38</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -484,10 +489,15 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>Sample Text</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>550e8400-e29b-41d4-a716-446655440000</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>example@example.com</t>
         </is>
@@ -501,7 +511,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-12-24 20:06:31</t>
+          <t>2026-01-05 00:22:38</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -512,10 +522,15 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>Sample Text</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>550e8400-e29b-41d4-a716-446655440000</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>example@example.com</t>
         </is>
@@ -529,7 +544,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-12-24 20:06:31</t>
+          <t>2026-01-05 00:22:38</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -540,10 +555,15 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>Sample Text</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>550e8400-e29b-41d4-a716-446655440000</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>example@example.com</t>
         </is>

</xml_diff>